<commit_message>
20200623 finished acquiring general trade figures part
</commit_message>
<xml_diff>
--- a/workflow.xlsx
+++ b/workflow.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\tradestat_enhanced\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\viwong\Desktop\tradestat_enhanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6CACA4E-43CE-4276-AF77-EB87DB7032A2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5612D782-69B2-43AE-8911-B19E3F12FAD0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="2070" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="552" windowWidth="16368" windowHeight="9612" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t xml:space="preserve"> Create a database using SQLite</t>
   </si>
@@ -73,6 +73,27 @@
   </si>
   <si>
     <t>product_code(sitc, hs items)</t>
+  </si>
+  <si>
+    <t>acquire hsccit, hscoit, hscoccit data respectively with periods assigned</t>
+  </si>
+  <si>
+    <t>merge them</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>for country</t>
+  </si>
+  <si>
+    <t>TX, DX, RX, IM by product ranking (one period)</t>
+  </si>
+  <si>
+    <t>general_trade figures, ranking (multiple periods)</t>
   </si>
 </sst>
 </file>
@@ -108,13 +129,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -396,191 +420,250 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D14" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="39.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="5.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.44140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="4.109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="40.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1"/>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1"/>
+      <c r="D2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="2">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
         <v>20200619</v>
       </c>
-      <c r="E2" s="2">
-        <v>20200621</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="F3" s="2">
+        <v>20200621</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2">
         <v>20200619</v>
       </c>
-      <c r="E3" s="2">
-        <v>20200621</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1">
-        <v>2</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="2">
-        <v>20200619</v>
-      </c>
-      <c r="E4" s="2">
-        <v>20200621</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="2">
+        <v>20200621</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>2</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="2">
-        <v>20200621</v>
-      </c>
-      <c r="E6" s="2">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>2</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="2">
+        <v>20200621</v>
+      </c>
+      <c r="F7" s="2">
+        <v>20200621</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2">
+        <v>2</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="2">
+        <v>20200621</v>
+      </c>
+      <c r="F8" s="2">
         <v>20200622</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>2</v>
-      </c>
-      <c r="B7" s="2">
-        <v>1</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="2">
-        <v>20200621</v>
-      </c>
-      <c r="E7" s="2">
-        <v>20200621</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>2</v>
-      </c>
-      <c r="B8" s="2">
-        <v>2</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="2">
-        <v>20200621</v>
-      </c>
-      <c r="E8" s="2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>2</v>
+      </c>
+      <c r="C9" s="2">
+        <v>3</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="2">
+        <v>20200621</v>
+      </c>
+      <c r="F9" s="2">
         <v>20200622</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>2</v>
-      </c>
-      <c r="B9" s="2">
-        <v>3</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="2">
-        <v>20200621</v>
-      </c>
-      <c r="E9" s="2">
-        <v>20200622</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>2</v>
       </c>
-      <c r="B10" s="2">
+      <c r="C10" s="2">
         <v>4</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="2">
-        <v>20200621</v>
-      </c>
       <c r="E10" s="2">
         <v>20200621</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="2">
+        <v>20200621</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>3</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>3</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="2">
+        <v>20200623</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C14" s="2">
+        <v>2</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="2">
+        <v>20200623</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>3</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C17" s="2">
+        <v>1</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="2">
+        <v>20200623</v>
+      </c>
+      <c r="F17" s="2">
+        <v>20200623</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C18" s="2">
+        <v>2</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="2">
+        <v>20200623</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
         <v>4</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D21" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
         <v>5</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D23" s="3" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finished general_trade figures, ranking (multiple periods)
</commit_message>
<xml_diff>
--- a/workflow.xlsx
+++ b/workflow.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\viwong\Desktop\tradestat_enhanced\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oda\OneDrive\文件\Github\tradestat_enhanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D8CC2EE-48BD-4726-80AE-73014AD8D8C1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5B5CE1E-D11B-4853-A19C-F6AE12A701E3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="17496" windowHeight="10416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -426,7 +426,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E23" sqref="E23"/>
+      <selection pane="bottomRight" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -637,7 +637,7 @@
         <v>20200623</v>
       </c>
       <c r="F17" s="2">
-        <v>20200623</v>
+        <v>20200626</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
prepare for R1 excel format
</commit_message>
<xml_diff>
--- a/workflow.xlsx
+++ b/workflow.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\tradestat_enhanced\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oda\OneDrive\文件\Github\tradestat_enhanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB32638E-3B85-41C7-B791-D9FD0B959738}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39217499-4F46-428E-83F4-4BAE1C735A21}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="17496" windowHeight="10416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t xml:space="preserve"> Create a database using SQLite</t>
   </si>
@@ -106,6 +106,15 @@
   </si>
   <si>
     <t>top X products, others (figures, %share, %change)</t>
+  </si>
+  <si>
+    <t>no need</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>excel formating</t>
   </si>
 </sst>
 </file>
@@ -432,27 +441,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomRight" activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="4.140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="40.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.44140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="4.109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="40.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="7" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -469,7 +478,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -479,7 +488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -497,7 +506,7 @@
         <v>20200621</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -515,7 +524,7 @@
         <v>20200621</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -523,7 +532,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>2</v>
       </c>
@@ -540,7 +549,7 @@
         <v>20200621</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>2</v>
       </c>
@@ -557,7 +566,7 @@
         <v>20200622</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>2</v>
       </c>
@@ -574,7 +583,7 @@
         <v>20200622</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>2</v>
       </c>
@@ -591,7 +600,7 @@
         <v>20200621</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>3</v>
       </c>
@@ -599,7 +608,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>3</v>
       </c>
@@ -619,7 +628,7 @@
         <v>20200626</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C14" s="2">
         <v>2</v>
       </c>
@@ -633,7 +642,7 @@
         <v>20200626</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>3</v>
       </c>
@@ -644,7 +653,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C17" s="2">
         <v>1</v>
       </c>
@@ -658,7 +667,7 @@
         <v>20200626</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C18" s="2">
         <v>2</v>
       </c>
@@ -666,13 +675,16 @@
         <v>22</v>
       </c>
       <c r="E18" s="2">
-        <v>20200623</v>
+        <v>20200703</v>
       </c>
       <c r="F18" s="2">
-        <v>20200701</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>20200705</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>4</v>
       </c>
@@ -680,7 +692,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
         <v>18</v>
       </c>
@@ -690,13 +702,16 @@
       <c r="D22" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E22" s="2">
+        <v>20200623</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D24" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
         <v>19</v>
       </c>
@@ -706,20 +721,45 @@
       <c r="D25" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="E25" s="2">
+        <v>20200703</v>
+      </c>
+      <c r="F25" s="2">
+        <v>20200705</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C26" s="2">
         <v>2</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
+      <c r="E26" s="2">
+        <v>20200703</v>
+      </c>
+      <c r="F26" s="2">
+        <v>20200705</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D28" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B29" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
         <v>5</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D34" s="3" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finished R1 upper part general trade figures, %chg, ranking
</commit_message>
<xml_diff>
--- a/workflow.xlsx
+++ b/workflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oda\OneDrive\文件\Github\tradestat_enhanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39217499-4F46-428E-83F4-4BAE1C735A21}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08F0AE29-BD1B-4F69-A012-B4EAEE5C8BA3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="17496" windowHeight="10416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t xml:space="preserve"> Create a database using SQLite</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>excel formating</t>
+  </si>
+  <si>
+    <t>upper part table(General trade figures, % change, rank)</t>
   </si>
 </sst>
 </file>
@@ -444,10 +447,10 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D29" sqref="D29"/>
+      <selection pane="bottomRight" activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -747,12 +750,21 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B29" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C29" s="2">
         <v>1</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E29" s="2">
+        <v>20200708</v>
+      </c>
+      <c r="F29" s="2">
+        <v>20200708</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>